<commit_message>
Aug 21 Case 003
Reconciled p and s numbering differences and annotated KAG version.
Updated metrics showing results for 003.
</commit_message>
<xml_diff>
--- a/Testing/DBvKG Comparison.xlsx
+++ b/Testing/DBvKG Comparison.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gradyke/Documents/GitHub/LegalTreebankDev/Case Processing/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gradyke/Documents/GitHub/LegalTreebankDev/Testing/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="7700" yWindow="1420" windowWidth="38820" windowHeight="19720" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="61260" yWindow="460" windowWidth="38820" windowHeight="19720" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="4" r:id="rId1"/>
@@ -21,6 +21,8 @@
     <definedName name="_000002_DDB" localSheetId="2">'000002'!$D$2:$E$152</definedName>
     <definedName name="_000002_KAG" localSheetId="2">'000002'!$A$2:$B$152</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'000001'!$C$1:$C$212</definedName>
+    <definedName name="DDB_1" localSheetId="3">'000003'!$D$2:$E$188</definedName>
+    <definedName name="KAG_1" localSheetId="3">'000003'!$A$2:$B$188</definedName>
   </definedNames>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -37,7 +39,7 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <connection id="1" name="000002 DDB" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" sourceFile="/Users/gradyke/Documents/GitHub/LegalTreebankDev/Testing/000002 DDB.csv" comma="1">
+    <textPr fileType="mac" sourceFile="/Users/gradyke/Documents/GitHub/LegalTreebankDev/Testing/000002 DDB.csv" comma="1">
       <textFields count="2">
         <textField/>
         <textField/>
@@ -45,7 +47,23 @@
     </textPr>
   </connection>
   <connection id="2" name="000002 KAG" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" sourceFile="/Users/gradyke/Documents/GitHub/LegalTreebankDev/Testing/000002 KAG.csv" comma="1">
+    <textPr fileType="mac" sourceFile="/Users/gradyke/Documents/GitHub/LegalTreebankDev/Testing/000002 KAG.csv" comma="1">
+      <textFields count="2">
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="3" name="DDB" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" codePage="10000" sourceFile="/Users/gradyke/Documents/GitHub/LegalTreebankDev/Testing/DDB.csv" comma="1">
+      <textFields count="2">
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="4" name="KAG" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" codePage="10000" sourceFile="/Users/gradyke/Documents/GitHub/LegalTreebankDev/Testing/KAG.csv" comma="1">
       <textFields count="2">
         <textField/>
         <textField/>
@@ -56,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="852" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1280" uniqueCount="35">
   <si>
     <t xml:space="preserve"> procedure</t>
   </si>
@@ -155,6 +173,12 @@
   </si>
   <si>
     <t>DDB</t>
+  </si>
+  <si>
+    <t>issue</t>
+  </si>
+  <si>
+    <t>analysis</t>
   </si>
 </sst>
 </file>
@@ -257,6 +281,14 @@
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="000002 KAG" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DDB_1" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="KAG_1" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7046,8 +7078,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="184" zoomScaleNormal="184" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+    <sheetView topLeftCell="A146" zoomScale="184" zoomScaleNormal="184" workbookViewId="0">
+      <selection activeCell="G153" sqref="G153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7231,7 +7263,7 @@
         <v>59</v>
       </c>
       <c r="K7" s="4">
-        <f>J7/$J$2</f>
+        <f t="shared" ref="K7:K13" si="0">J7/$J$2</f>
         <v>0.39072847682119205</v>
       </c>
     </row>
@@ -7262,7 +7294,7 @@
         <v>29</v>
       </c>
       <c r="K8" s="4">
-        <f>J8/$J$2</f>
+        <f t="shared" si="0"/>
         <v>0.19205298013245034</v>
       </c>
     </row>
@@ -7293,7 +7325,7 @@
         <v>5</v>
       </c>
       <c r="K9" s="4">
-        <f>J9/$J$2</f>
+        <f t="shared" si="0"/>
         <v>3.3112582781456956E-2</v>
       </c>
     </row>
@@ -7324,7 +7356,7 @@
         <v>27</v>
       </c>
       <c r="K10" s="4">
-        <f>J10/$J$2</f>
+        <f t="shared" si="0"/>
         <v>0.17880794701986755</v>
       </c>
     </row>
@@ -7355,7 +7387,7 @@
         <v>3</v>
       </c>
       <c r="K11" s="4">
-        <f>J11/$J$2</f>
+        <f t="shared" si="0"/>
         <v>1.9867549668874173E-2</v>
       </c>
     </row>
@@ -7386,7 +7418,7 @@
         <v>10</v>
       </c>
       <c r="K12" s="4">
-        <f>J12/$J$2</f>
+        <f t="shared" si="0"/>
         <v>6.6225165562913912E-2</v>
       </c>
     </row>
@@ -7417,7 +7449,7 @@
         <v>18</v>
       </c>
       <c r="K13" s="4">
-        <f>J13/$J$2</f>
+        <f t="shared" si="0"/>
         <v>0.11920529801324503</v>
       </c>
     </row>
@@ -7521,7 +7553,7 @@
         <v>36</v>
       </c>
       <c r="K17" s="4">
-        <f t="shared" ref="K17:K23" si="0">J17/210</f>
+        <f t="shared" ref="K17:K23" si="1">J17/210</f>
         <v>0.17142857142857143</v>
       </c>
     </row>
@@ -7552,7 +7584,7 @@
         <v>38</v>
       </c>
       <c r="K18" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.18095238095238095</v>
       </c>
     </row>
@@ -7583,7 +7615,7 @@
         <v>16</v>
       </c>
       <c r="K19" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7.6190476190476197E-2</v>
       </c>
     </row>
@@ -7614,7 +7646,7 @@
         <v>29</v>
       </c>
       <c r="K20" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.1380952380952381</v>
       </c>
     </row>
@@ -7645,7 +7677,7 @@
         <v>4</v>
       </c>
       <c r="K21" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.9047619047619049E-2</v>
       </c>
     </row>
@@ -7676,7 +7708,7 @@
         <v>11</v>
       </c>
       <c r="K22" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5.2380952380952382E-2</v>
       </c>
     </row>
@@ -7707,7 +7739,7 @@
         <v>17</v>
       </c>
       <c r="K23" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8.0952380952380956E-2</v>
       </c>
     </row>
@@ -10409,14 +10441,4090 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:K189"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E43" sqref="E43"/>
+    <sheetView tabSelected="1" zoomScale="132" zoomScaleNormal="132" workbookViewId="0">
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" style="1"/>
+    <col min="4" max="4" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" style="1"/>
+    <col min="9" max="9" width="15.83203125" customWidth="1"/>
+    <col min="11" max="11" width="16.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K1" s="4"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1">
+        <v>6</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="1">
+        <v>6</v>
+      </c>
+      <c r="I2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2">
+        <v>187</v>
+      </c>
+      <c r="K2" s="4"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="1">
+        <v>3</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="1">
+        <v>3</v>
+      </c>
+      <c r="I3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J3">
+        <v>29</v>
+      </c>
+      <c r="K3" s="4"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1">
+        <v>6</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F4" s="1">
+        <v>6</v>
+      </c>
+      <c r="I4" t="s">
+        <v>14</v>
+      </c>
+      <c r="J4">
+        <f>(J2-J3)/J2</f>
+        <v>0.84491978609625673</v>
+      </c>
+      <c r="K4" s="4"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="1">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="E5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" s="1">
+        <v>2</v>
+      </c>
+      <c r="K5" s="4"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="1">
+        <v>6</v>
+      </c>
+      <c r="D6">
+        <v>5</v>
+      </c>
+      <c r="E6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F6" s="1">
+        <v>6</v>
+      </c>
+      <c r="I6" t="s">
+        <v>15</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" s="1">
+        <v>6</v>
+      </c>
+      <c r="D7">
+        <v>6</v>
+      </c>
+      <c r="E7" t="s">
+        <v>0</v>
+      </c>
+      <c r="F7" s="1">
+        <v>6</v>
+      </c>
+      <c r="I7" t="s">
+        <v>16</v>
+      </c>
+      <c r="J7">
+        <f>COUNTIF(C2:C188,C16)</f>
+        <v>63</v>
+      </c>
+      <c r="K7" s="4">
+        <f t="shared" ref="K7:K13" si="0">J7/$J$2</f>
+        <v>0.33689839572192515</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="1">
+        <v>7</v>
+      </c>
+      <c r="D8">
+        <v>7</v>
+      </c>
+      <c r="E8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8" s="1">
+        <v>1</v>
+      </c>
+      <c r="G8" t="s">
+        <v>9</v>
+      </c>
+      <c r="I8" t="s">
+        <v>17</v>
+      </c>
+      <c r="J8">
+        <f>COUNTIF(C2:C188,C12)</f>
+        <v>77</v>
+      </c>
+      <c r="K8" s="4">
+        <f t="shared" si="0"/>
+        <v>0.41176470588235292</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="1">
+        <v>7</v>
+      </c>
+      <c r="D9">
+        <v>8</v>
+      </c>
+      <c r="E9" t="s">
+        <v>5</v>
+      </c>
+      <c r="F9" s="1">
+        <v>7</v>
+      </c>
+      <c r="I9" t="s">
+        <v>18</v>
+      </c>
+      <c r="J9">
+        <f>COUNTIF(C2:C188,C3)</f>
+        <v>10</v>
+      </c>
+      <c r="K9" s="4">
+        <f t="shared" si="0"/>
+        <v>5.3475935828877004E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="1">
+        <v>7</v>
+      </c>
+      <c r="D10">
+        <v>9</v>
+      </c>
+      <c r="E10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F10" s="1">
+        <v>7</v>
+      </c>
+      <c r="I10" t="s">
+        <v>19</v>
+      </c>
+      <c r="J10">
+        <f>COUNTIF(C2:C188,C14)</f>
+        <v>10</v>
+      </c>
+      <c r="K10" s="4">
+        <f t="shared" si="0"/>
+        <v>5.3475935828877004E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="1">
+        <v>7</v>
+      </c>
+      <c r="D11">
+        <v>10</v>
+      </c>
+      <c r="E11" t="s">
+        <v>5</v>
+      </c>
+      <c r="F11" s="1">
+        <v>7</v>
+      </c>
+      <c r="I11" t="s">
+        <v>20</v>
+      </c>
+      <c r="J11">
+        <f>COUNTIF(C2:C188,C81)</f>
+        <v>2</v>
+      </c>
+      <c r="K11" s="4">
+        <f t="shared" si="0"/>
+        <v>1.06951871657754E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" s="1">
+        <v>2</v>
+      </c>
+      <c r="D12">
+        <v>11</v>
+      </c>
+      <c r="E12" t="s">
+        <v>2</v>
+      </c>
+      <c r="F12" s="1">
+        <v>2</v>
+      </c>
+      <c r="I12" t="s">
+        <v>21</v>
+      </c>
+      <c r="J12">
+        <f>COUNTIF(C2:C188,C6)</f>
+        <v>5</v>
+      </c>
+      <c r="K12" s="4">
+        <f t="shared" si="0"/>
+        <v>2.6737967914438502E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="1">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>12</v>
+      </c>
+      <c r="E13" t="s">
+        <v>2</v>
+      </c>
+      <c r="F13" s="1">
+        <v>2</v>
+      </c>
+      <c r="G13" t="s">
+        <v>9</v>
+      </c>
+      <c r="I13" t="s">
+        <v>22</v>
+      </c>
+      <c r="J13">
+        <f>COUNTIF(C2:C188,C9)</f>
+        <v>20</v>
+      </c>
+      <c r="K13" s="4">
+        <f t="shared" si="0"/>
+        <v>0.10695187165775401</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="1">
+        <v>4</v>
+      </c>
+      <c r="D14">
+        <v>13</v>
+      </c>
+      <c r="E14" t="s">
+        <v>3</v>
+      </c>
+      <c r="F14" s="1">
+        <v>4</v>
+      </c>
+      <c r="J14">
+        <f>SUM(J7:J13)</f>
+        <v>187</v>
+      </c>
+      <c r="K14" s="4">
+        <f>PRODUCT(K7:K13)</f>
+        <v>1.213305103970621E-8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" s="1">
+        <v>4</v>
+      </c>
+      <c r="D15">
+        <v>14</v>
+      </c>
+      <c r="E15" t="s">
+        <v>3</v>
+      </c>
+      <c r="F15" s="1">
+        <v>4</v>
+      </c>
+      <c r="K15" s="4"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" s="1">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>15</v>
+      </c>
+      <c r="E16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F16" s="1">
+        <v>3</v>
+      </c>
+      <c r="G16" t="s">
+        <v>9</v>
+      </c>
+      <c r="I16" t="s">
+        <v>23</v>
+      </c>
+      <c r="K16" s="4"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="1">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>16</v>
+      </c>
+      <c r="E17" t="s">
+        <v>0</v>
+      </c>
+      <c r="F17" s="1">
+        <v>6</v>
+      </c>
+      <c r="G17" t="s">
+        <v>9</v>
+      </c>
+      <c r="I17" t="s">
+        <v>16</v>
+      </c>
+      <c r="J17">
+        <f>COUNTIF(F2:F188,F8)</f>
+        <v>56</v>
+      </c>
+      <c r="K17" s="4">
+        <f t="shared" ref="K17:K23" si="1">J17/210</f>
+        <v>0.26666666666666666</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>2</v>
+      </c>
+      <c r="C18" s="1">
+        <v>2</v>
+      </c>
+      <c r="D18">
+        <v>17</v>
+      </c>
+      <c r="E18" t="s">
+        <v>2</v>
+      </c>
+      <c r="F18" s="1">
+        <v>2</v>
+      </c>
+      <c r="I18" t="s">
+        <v>17</v>
+      </c>
+      <c r="J18">
+        <f>COUNTIF(F2:F188,F5)</f>
+        <v>80</v>
+      </c>
+      <c r="K18" s="4">
+        <f t="shared" si="1"/>
+        <v>0.38095238095238093</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>2</v>
+      </c>
+      <c r="C19" s="1">
+        <v>2</v>
+      </c>
+      <c r="D19">
+        <v>18</v>
+      </c>
+      <c r="E19" t="s">
+        <v>2</v>
+      </c>
+      <c r="F19" s="1">
+        <v>2</v>
+      </c>
+      <c r="I19" t="s">
+        <v>18</v>
+      </c>
+      <c r="J19">
+        <f>COUNTIF(F2:F188,F3)</f>
+        <v>21</v>
+      </c>
+      <c r="K19" s="4">
+        <f t="shared" si="1"/>
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>2</v>
+      </c>
+      <c r="C20" s="1">
+        <v>2</v>
+      </c>
+      <c r="D20">
+        <v>19</v>
+      </c>
+      <c r="E20" t="s">
+        <v>2</v>
+      </c>
+      <c r="F20" s="1">
+        <v>2</v>
+      </c>
+      <c r="I20" t="s">
+        <v>19</v>
+      </c>
+      <c r="J20">
+        <f>COUNTIF(F2:F188,F14)</f>
+        <v>11</v>
+      </c>
+      <c r="K20" s="4">
+        <f t="shared" si="1"/>
+        <v>5.2380952380952382E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>2</v>
+      </c>
+      <c r="C21" s="1">
+        <v>2</v>
+      </c>
+      <c r="D21">
+        <v>20</v>
+      </c>
+      <c r="E21" t="s">
+        <v>2</v>
+      </c>
+      <c r="F21" s="1">
+        <v>2</v>
+      </c>
+      <c r="I21" t="s">
+        <v>20</v>
+      </c>
+      <c r="J21">
+        <f>COUNTIF(F2:F188,F165)</f>
+        <v>2</v>
+      </c>
+      <c r="K21" s="4">
+        <f t="shared" si="1"/>
+        <v>9.5238095238095247E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>2</v>
+      </c>
+      <c r="C22" s="1">
+        <v>2</v>
+      </c>
+      <c r="D22">
+        <v>21</v>
+      </c>
+      <c r="E22" t="s">
+        <v>2</v>
+      </c>
+      <c r="F22" s="1">
+        <v>2</v>
+      </c>
+      <c r="I22" t="s">
+        <v>21</v>
+      </c>
+      <c r="J22">
+        <f>COUNTIF(F2:F188,F17)</f>
+        <v>6</v>
+      </c>
+      <c r="K22" s="4">
+        <f t="shared" si="1"/>
+        <v>2.8571428571428571E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>2</v>
+      </c>
+      <c r="C23" s="1">
+        <v>2</v>
+      </c>
+      <c r="D23">
+        <v>22</v>
+      </c>
+      <c r="E23" t="s">
+        <v>2</v>
+      </c>
+      <c r="F23" s="1">
+        <v>2</v>
+      </c>
+      <c r="I23" t="s">
+        <v>22</v>
+      </c>
+      <c r="J23">
+        <f>COUNTIF(F2:F188,F11)</f>
+        <v>11</v>
+      </c>
+      <c r="K23" s="4">
+        <f t="shared" si="1"/>
+        <v>5.2380952380952382E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>2</v>
+      </c>
+      <c r="C24" s="1">
+        <v>2</v>
+      </c>
+      <c r="D24">
+        <v>23</v>
+      </c>
+      <c r="E24" t="s">
+        <v>2</v>
+      </c>
+      <c r="F24" s="1">
+        <v>2</v>
+      </c>
+      <c r="J24">
+        <f>SUM(J17:J23)</f>
+        <v>187</v>
+      </c>
+      <c r="K24" s="4">
+        <f>PRODUCT(K17:K23)</f>
+        <v>7.584533291414684E-9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>2</v>
+      </c>
+      <c r="C25" s="1">
+        <v>2</v>
+      </c>
+      <c r="D25">
+        <v>24</v>
+      </c>
+      <c r="E25" t="s">
+        <v>2</v>
+      </c>
+      <c r="F25" s="1">
+        <v>2</v>
+      </c>
+      <c r="K25" s="4"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>2</v>
+      </c>
+      <c r="C26" s="1">
+        <v>2</v>
+      </c>
+      <c r="D26">
+        <v>25</v>
+      </c>
+      <c r="E26" t="s">
+        <v>2</v>
+      </c>
+      <c r="F26" s="1">
+        <v>2</v>
+      </c>
+      <c r="I26" t="s">
+        <v>24</v>
+      </c>
+      <c r="K26" s="4">
+        <f>K14+K24</f>
+        <v>1.9717584331120894E-8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>2</v>
+      </c>
+      <c r="C27" s="1">
+        <v>2</v>
+      </c>
+      <c r="D27">
+        <v>26</v>
+      </c>
+      <c r="E27" t="s">
+        <v>2</v>
+      </c>
+      <c r="F27" s="1">
+        <v>2</v>
+      </c>
+      <c r="K27" s="4"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>2</v>
+      </c>
+      <c r="C28" s="1">
+        <v>2</v>
+      </c>
+      <c r="D28">
+        <v>27</v>
+      </c>
+      <c r="E28" t="s">
+        <v>2</v>
+      </c>
+      <c r="F28" s="1">
+        <v>2</v>
+      </c>
+      <c r="I28" t="s">
+        <v>25</v>
+      </c>
+      <c r="K28" s="4">
+        <f>(J4-K26)/(1-K26)</f>
+        <v>0.8449197830384495</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>2</v>
+      </c>
+      <c r="C29" s="1">
+        <v>2</v>
+      </c>
+      <c r="D29">
+        <v>28</v>
+      </c>
+      <c r="E29" t="s">
+        <v>2</v>
+      </c>
+      <c r="F29" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>2</v>
+      </c>
+      <c r="C30" s="1">
+        <v>2</v>
+      </c>
+      <c r="D30">
+        <v>29</v>
+      </c>
+      <c r="E30" t="s">
+        <v>2</v>
+      </c>
+      <c r="F30" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>2</v>
+      </c>
+      <c r="C31" s="1">
+        <v>2</v>
+      </c>
+      <c r="D31">
+        <v>30</v>
+      </c>
+      <c r="E31" t="s">
+        <v>2</v>
+      </c>
+      <c r="F31" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>2</v>
+      </c>
+      <c r="C32" s="1">
+        <v>2</v>
+      </c>
+      <c r="D32">
+        <v>31</v>
+      </c>
+      <c r="E32" t="s">
+        <v>2</v>
+      </c>
+      <c r="F32" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>2</v>
+      </c>
+      <c r="C33" s="1">
+        <v>2</v>
+      </c>
+      <c r="D33">
+        <v>32</v>
+      </c>
+      <c r="E33" t="s">
+        <v>2</v>
+      </c>
+      <c r="F33" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>2</v>
+      </c>
+      <c r="C34" s="1">
+        <v>2</v>
+      </c>
+      <c r="D34">
+        <v>33</v>
+      </c>
+      <c r="E34" t="s">
+        <v>2</v>
+      </c>
+      <c r="F34" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>2</v>
+      </c>
+      <c r="C35" s="1">
+        <v>2</v>
+      </c>
+      <c r="D35">
+        <v>34</v>
+      </c>
+      <c r="E35" t="s">
+        <v>2</v>
+      </c>
+      <c r="F35" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>2</v>
+      </c>
+      <c r="C36" s="1">
+        <v>2</v>
+      </c>
+      <c r="D36">
+        <v>35</v>
+      </c>
+      <c r="E36" t="s">
+        <v>2</v>
+      </c>
+      <c r="F36" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
+        <v>2</v>
+      </c>
+      <c r="C37" s="1">
+        <v>2</v>
+      </c>
+      <c r="D37">
+        <v>36</v>
+      </c>
+      <c r="E37" t="s">
+        <v>2</v>
+      </c>
+      <c r="F37" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
+        <v>2</v>
+      </c>
+      <c r="C38" s="1">
+        <v>2</v>
+      </c>
+      <c r="D38">
+        <v>37</v>
+      </c>
+      <c r="E38" t="s">
+        <v>2</v>
+      </c>
+      <c r="F38" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
+        <v>2</v>
+      </c>
+      <c r="C39" s="1">
+        <v>2</v>
+      </c>
+      <c r="D39">
+        <v>38</v>
+      </c>
+      <c r="E39" t="s">
+        <v>2</v>
+      </c>
+      <c r="F39" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40" t="s">
+        <v>2</v>
+      </c>
+      <c r="C40" s="1">
+        <v>2</v>
+      </c>
+      <c r="D40">
+        <v>39</v>
+      </c>
+      <c r="E40" t="s">
+        <v>2</v>
+      </c>
+      <c r="F40" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41" t="s">
+        <v>2</v>
+      </c>
+      <c r="C41" s="1">
+        <v>2</v>
+      </c>
+      <c r="D41">
+        <v>40</v>
+      </c>
+      <c r="E41" t="s">
+        <v>2</v>
+      </c>
+      <c r="F41" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42" t="s">
+        <v>2</v>
+      </c>
+      <c r="C42" s="1">
+        <v>2</v>
+      </c>
+      <c r="D42">
+        <v>41</v>
+      </c>
+      <c r="E42" t="s">
+        <v>2</v>
+      </c>
+      <c r="F42" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43" t="s">
+        <v>2</v>
+      </c>
+      <c r="C43" s="1">
+        <v>2</v>
+      </c>
+      <c r="D43">
+        <v>42</v>
+      </c>
+      <c r="E43" t="s">
+        <v>2</v>
+      </c>
+      <c r="F43" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44" t="s">
+        <v>2</v>
+      </c>
+      <c r="C44" s="1">
+        <v>2</v>
+      </c>
+      <c r="D44">
+        <v>43</v>
+      </c>
+      <c r="E44" t="s">
+        <v>2</v>
+      </c>
+      <c r="F44" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45" t="s">
+        <v>2</v>
+      </c>
+      <c r="C45" s="1">
+        <v>2</v>
+      </c>
+      <c r="D45">
+        <v>44</v>
+      </c>
+      <c r="E45" t="s">
+        <v>2</v>
+      </c>
+      <c r="F45" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46" t="s">
+        <v>2</v>
+      </c>
+      <c r="C46" s="1">
+        <v>2</v>
+      </c>
+      <c r="D46">
+        <v>45</v>
+      </c>
+      <c r="E46" t="s">
+        <v>2</v>
+      </c>
+      <c r="F46" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47" t="s">
+        <v>4</v>
+      </c>
+      <c r="C47" s="1">
+        <v>1</v>
+      </c>
+      <c r="D47">
+        <v>46</v>
+      </c>
+      <c r="E47" t="s">
+        <v>4</v>
+      </c>
+      <c r="F47" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48" t="s">
+        <v>4</v>
+      </c>
+      <c r="C48" s="1">
+        <v>1</v>
+      </c>
+      <c r="D48">
+        <v>47</v>
+      </c>
+      <c r="E48" t="s">
+        <v>4</v>
+      </c>
+      <c r="F48" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49" t="s">
+        <v>5</v>
+      </c>
+      <c r="C49" s="1">
+        <v>7</v>
+      </c>
+      <c r="D49">
+        <v>48</v>
+      </c>
+      <c r="E49" t="s">
+        <v>4</v>
+      </c>
+      <c r="F49" s="1">
+        <v>1</v>
+      </c>
+      <c r="G49" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50" t="s">
+        <v>4</v>
+      </c>
+      <c r="C50" s="1">
+        <v>1</v>
+      </c>
+      <c r="D50">
+        <v>49</v>
+      </c>
+      <c r="E50" t="s">
+        <v>2</v>
+      </c>
+      <c r="F50" s="1">
+        <v>2</v>
+      </c>
+      <c r="G50" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51" t="s">
+        <v>4</v>
+      </c>
+      <c r="C51" s="1">
+        <v>1</v>
+      </c>
+      <c r="D51">
+        <v>50</v>
+      </c>
+      <c r="E51" t="s">
+        <v>2</v>
+      </c>
+      <c r="F51" s="1">
+        <v>2</v>
+      </c>
+      <c r="G51" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52" t="s">
+        <v>4</v>
+      </c>
+      <c r="C52" s="1">
+        <v>1</v>
+      </c>
+      <c r="D52">
+        <v>51</v>
+      </c>
+      <c r="E52" t="s">
+        <v>4</v>
+      </c>
+      <c r="F52" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53" t="s">
+        <v>4</v>
+      </c>
+      <c r="C53" s="1">
+        <v>1</v>
+      </c>
+      <c r="D53">
+        <v>52</v>
+      </c>
+      <c r="E53" t="s">
+        <v>4</v>
+      </c>
+      <c r="F53" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54" t="s">
+        <v>4</v>
+      </c>
+      <c r="C54" s="1">
+        <v>1</v>
+      </c>
+      <c r="D54">
+        <v>53</v>
+      </c>
+      <c r="E54" t="s">
+        <v>4</v>
+      </c>
+      <c r="F54" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55" t="s">
+        <v>6</v>
+      </c>
+      <c r="C55" s="1">
+        <v>3</v>
+      </c>
+      <c r="D55">
+        <v>54</v>
+      </c>
+      <c r="E55" t="s">
+        <v>6</v>
+      </c>
+      <c r="F55" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56" t="s">
+        <v>3</v>
+      </c>
+      <c r="C56" s="1">
+        <v>4</v>
+      </c>
+      <c r="D56">
+        <v>55</v>
+      </c>
+      <c r="E56" t="s">
+        <v>3</v>
+      </c>
+      <c r="F56" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57" t="s">
+        <v>3</v>
+      </c>
+      <c r="C57" s="1">
+        <v>4</v>
+      </c>
+      <c r="D57">
+        <v>56</v>
+      </c>
+      <c r="E57" t="s">
+        <v>3</v>
+      </c>
+      <c r="F57" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58" t="s">
+        <v>3</v>
+      </c>
+      <c r="C58" s="1">
+        <v>4</v>
+      </c>
+      <c r="D58">
+        <v>57</v>
+      </c>
+      <c r="E58" t="s">
+        <v>3</v>
+      </c>
+      <c r="F58" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59" t="s">
+        <v>4</v>
+      </c>
+      <c r="C59" s="1">
+        <v>1</v>
+      </c>
+      <c r="D59">
+        <v>58</v>
+      </c>
+      <c r="E59" t="s">
+        <v>6</v>
+      </c>
+      <c r="F59" s="1">
+        <v>3</v>
+      </c>
+      <c r="G59" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60" t="s">
+        <v>5</v>
+      </c>
+      <c r="C60" s="1">
+        <v>7</v>
+      </c>
+      <c r="D60">
+        <v>59</v>
+      </c>
+      <c r="E60" t="s">
+        <v>5</v>
+      </c>
+      <c r="F60" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="B61" t="s">
+        <v>5</v>
+      </c>
+      <c r="C61" s="1">
+        <v>7</v>
+      </c>
+      <c r="D61">
+        <v>60</v>
+      </c>
+      <c r="E61" t="s">
+        <v>5</v>
+      </c>
+      <c r="F61" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <v>61</v>
+      </c>
+      <c r="B62" t="s">
+        <v>5</v>
+      </c>
+      <c r="C62" s="1">
+        <v>7</v>
+      </c>
+      <c r="D62">
+        <v>61</v>
+      </c>
+      <c r="E62" t="s">
+        <v>4</v>
+      </c>
+      <c r="F62" s="1">
+        <v>1</v>
+      </c>
+      <c r="G62" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <v>62</v>
+      </c>
+      <c r="B63" t="s">
+        <v>5</v>
+      </c>
+      <c r="C63" s="1">
+        <v>7</v>
+      </c>
+      <c r="D63">
+        <v>62</v>
+      </c>
+      <c r="E63" t="s">
+        <v>4</v>
+      </c>
+      <c r="F63" s="1">
+        <v>1</v>
+      </c>
+      <c r="G63" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A64">
+        <v>63</v>
+      </c>
+      <c r="B64" t="s">
+        <v>4</v>
+      </c>
+      <c r="C64" s="1">
+        <v>1</v>
+      </c>
+      <c r="D64">
+        <v>63</v>
+      </c>
+      <c r="E64" t="s">
+        <v>4</v>
+      </c>
+      <c r="F64" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A65">
+        <v>64</v>
+      </c>
+      <c r="B65" t="s">
+        <v>5</v>
+      </c>
+      <c r="C65" s="1">
+        <v>7</v>
+      </c>
+      <c r="D65">
+        <v>64</v>
+      </c>
+      <c r="E65" t="s">
+        <v>4</v>
+      </c>
+      <c r="F65" s="1">
+        <v>1</v>
+      </c>
+      <c r="G65" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A66">
+        <v>65</v>
+      </c>
+      <c r="B66" t="s">
+        <v>5</v>
+      </c>
+      <c r="C66" s="1">
+        <v>7</v>
+      </c>
+      <c r="D66">
+        <v>65</v>
+      </c>
+      <c r="E66" t="s">
+        <v>4</v>
+      </c>
+      <c r="F66" s="1">
+        <v>1</v>
+      </c>
+      <c r="G66" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A67">
+        <v>66</v>
+      </c>
+      <c r="B67" t="s">
+        <v>4</v>
+      </c>
+      <c r="C67" s="1">
+        <v>1</v>
+      </c>
+      <c r="D67">
+        <v>66</v>
+      </c>
+      <c r="E67" t="s">
+        <v>4</v>
+      </c>
+      <c r="F67" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A68">
+        <v>67</v>
+      </c>
+      <c r="B68" t="s">
+        <v>5</v>
+      </c>
+      <c r="C68" s="1">
+        <v>7</v>
+      </c>
+      <c r="D68">
+        <v>67</v>
+      </c>
+      <c r="E68" t="s">
+        <v>5</v>
+      </c>
+      <c r="F68" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A69">
+        <v>68</v>
+      </c>
+      <c r="B69" t="s">
+        <v>4</v>
+      </c>
+      <c r="C69" s="1">
+        <v>1</v>
+      </c>
+      <c r="D69">
+        <v>68</v>
+      </c>
+      <c r="E69" t="s">
+        <v>6</v>
+      </c>
+      <c r="F69" s="1">
+        <v>3</v>
+      </c>
+      <c r="G69" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A70">
+        <v>69</v>
+      </c>
+      <c r="B70" t="s">
+        <v>4</v>
+      </c>
+      <c r="C70" s="1">
+        <v>1</v>
+      </c>
+      <c r="D70">
+        <v>69</v>
+      </c>
+      <c r="E70" t="s">
+        <v>6</v>
+      </c>
+      <c r="F70" s="1">
+        <v>3</v>
+      </c>
+      <c r="G70" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A71">
+        <v>70</v>
+      </c>
+      <c r="B71" t="s">
+        <v>6</v>
+      </c>
+      <c r="C71" s="1">
+        <v>3</v>
+      </c>
+      <c r="D71">
+        <v>70</v>
+      </c>
+      <c r="E71" t="s">
+        <v>6</v>
+      </c>
+      <c r="F71" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A72">
+        <v>71</v>
+      </c>
+      <c r="B72" t="s">
+        <v>4</v>
+      </c>
+      <c r="C72" s="1">
+        <v>1</v>
+      </c>
+      <c r="D72">
+        <v>71</v>
+      </c>
+      <c r="E72" t="s">
+        <v>4</v>
+      </c>
+      <c r="F72" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A73">
+        <v>72</v>
+      </c>
+      <c r="B73" t="s">
+        <v>4</v>
+      </c>
+      <c r="C73" s="1">
+        <v>1</v>
+      </c>
+      <c r="D73">
+        <v>72</v>
+      </c>
+      <c r="E73" t="s">
+        <v>4</v>
+      </c>
+      <c r="F73" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A74">
+        <v>73</v>
+      </c>
+      <c r="B74" t="s">
+        <v>5</v>
+      </c>
+      <c r="C74" s="1">
+        <v>7</v>
+      </c>
+      <c r="D74">
+        <v>73</v>
+      </c>
+      <c r="E74" t="s">
+        <v>5</v>
+      </c>
+      <c r="F74" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A75">
+        <v>74</v>
+      </c>
+      <c r="B75" t="s">
+        <v>4</v>
+      </c>
+      <c r="C75" s="1">
+        <v>1</v>
+      </c>
+      <c r="D75">
+        <v>74</v>
+      </c>
+      <c r="E75" t="s">
+        <v>4</v>
+      </c>
+      <c r="F75" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A76">
+        <v>75</v>
+      </c>
+      <c r="B76" t="s">
+        <v>4</v>
+      </c>
+      <c r="C76" s="1">
+        <v>1</v>
+      </c>
+      <c r="D76">
+        <v>75</v>
+      </c>
+      <c r="E76" t="s">
+        <v>4</v>
+      </c>
+      <c r="F76" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A77">
+        <v>76</v>
+      </c>
+      <c r="B77" t="s">
+        <v>4</v>
+      </c>
+      <c r="C77" s="1">
+        <v>1</v>
+      </c>
+      <c r="D77">
+        <v>76</v>
+      </c>
+      <c r="E77" t="s">
+        <v>34</v>
+      </c>
+      <c r="F77" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A78">
+        <v>77</v>
+      </c>
+      <c r="B78" t="s">
+        <v>5</v>
+      </c>
+      <c r="C78" s="1">
+        <v>7</v>
+      </c>
+      <c r="D78">
+        <v>77</v>
+      </c>
+      <c r="E78" t="s">
+        <v>5</v>
+      </c>
+      <c r="F78" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A79">
+        <v>78</v>
+      </c>
+      <c r="B79" t="s">
+        <v>5</v>
+      </c>
+      <c r="C79" s="1">
+        <v>7</v>
+      </c>
+      <c r="D79">
+        <v>78</v>
+      </c>
+      <c r="E79" t="s">
+        <v>5</v>
+      </c>
+      <c r="F79" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A80">
+        <v>79</v>
+      </c>
+      <c r="B80" t="s">
+        <v>5</v>
+      </c>
+      <c r="C80" s="1">
+        <v>7</v>
+      </c>
+      <c r="D80">
+        <v>79</v>
+      </c>
+      <c r="E80" t="s">
+        <v>5</v>
+      </c>
+      <c r="F80" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A81">
+        <v>80</v>
+      </c>
+      <c r="B81" t="s">
+        <v>1</v>
+      </c>
+      <c r="C81" s="1">
+        <v>5</v>
+      </c>
+      <c r="D81">
+        <v>80</v>
+      </c>
+      <c r="E81" t="s">
+        <v>1</v>
+      </c>
+      <c r="F81" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A82">
+        <v>81</v>
+      </c>
+      <c r="B82" t="s">
+        <v>2</v>
+      </c>
+      <c r="C82" s="1">
+        <v>2</v>
+      </c>
+      <c r="D82">
+        <v>81</v>
+      </c>
+      <c r="E82" t="s">
+        <v>2</v>
+      </c>
+      <c r="F82" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A83">
+        <v>82</v>
+      </c>
+      <c r="B83" t="s">
+        <v>2</v>
+      </c>
+      <c r="C83" s="1">
+        <v>2</v>
+      </c>
+      <c r="D83">
+        <v>82</v>
+      </c>
+      <c r="E83" t="s">
+        <v>4</v>
+      </c>
+      <c r="F83" s="1">
+        <v>1</v>
+      </c>
+      <c r="G83" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A84">
+        <v>83</v>
+      </c>
+      <c r="B84" t="s">
+        <v>4</v>
+      </c>
+      <c r="C84" s="1">
+        <v>1</v>
+      </c>
+      <c r="D84">
+        <v>83</v>
+      </c>
+      <c r="E84" t="s">
+        <v>4</v>
+      </c>
+      <c r="F84" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A85">
+        <v>84</v>
+      </c>
+      <c r="B85" t="s">
+        <v>5</v>
+      </c>
+      <c r="C85" s="1">
+        <v>7</v>
+      </c>
+      <c r="D85">
+        <v>84</v>
+      </c>
+      <c r="E85" t="s">
+        <v>5</v>
+      </c>
+      <c r="F85" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A86">
+        <v>85</v>
+      </c>
+      <c r="B86" t="s">
+        <v>5</v>
+      </c>
+      <c r="C86" s="1">
+        <v>7</v>
+      </c>
+      <c r="D86">
+        <v>85</v>
+      </c>
+      <c r="E86" t="s">
+        <v>4</v>
+      </c>
+      <c r="F86" s="1">
+        <v>1</v>
+      </c>
+      <c r="G86" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A87">
+        <v>86</v>
+      </c>
+      <c r="B87" t="s">
+        <v>5</v>
+      </c>
+      <c r="C87" s="1">
+        <v>7</v>
+      </c>
+      <c r="D87">
+        <v>86</v>
+      </c>
+      <c r="E87" t="s">
+        <v>4</v>
+      </c>
+      <c r="F87" s="1">
+        <v>1</v>
+      </c>
+      <c r="G87" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A88">
+        <v>87</v>
+      </c>
+      <c r="B88" t="s">
+        <v>4</v>
+      </c>
+      <c r="C88" s="1">
+        <v>1</v>
+      </c>
+      <c r="D88">
+        <v>87</v>
+      </c>
+      <c r="E88" t="s">
+        <v>4</v>
+      </c>
+      <c r="F88" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A89">
+        <v>88</v>
+      </c>
+      <c r="B89" t="s">
+        <v>2</v>
+      </c>
+      <c r="C89" s="1">
+        <v>2</v>
+      </c>
+      <c r="D89">
+        <v>88</v>
+      </c>
+      <c r="E89" t="s">
+        <v>2</v>
+      </c>
+      <c r="F89" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A90">
+        <v>89</v>
+      </c>
+      <c r="B90" t="s">
+        <v>2</v>
+      </c>
+      <c r="C90" s="1">
+        <v>2</v>
+      </c>
+      <c r="D90">
+        <v>89</v>
+      </c>
+      <c r="E90" t="s">
+        <v>2</v>
+      </c>
+      <c r="F90" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A91">
+        <v>90</v>
+      </c>
+      <c r="B91" t="s">
+        <v>2</v>
+      </c>
+      <c r="C91" s="1">
+        <v>2</v>
+      </c>
+      <c r="D91">
+        <v>90</v>
+      </c>
+      <c r="E91" t="s">
+        <v>2</v>
+      </c>
+      <c r="F91" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A92">
+        <v>91</v>
+      </c>
+      <c r="B92" t="s">
+        <v>2</v>
+      </c>
+      <c r="C92" s="1">
+        <v>2</v>
+      </c>
+      <c r="D92">
+        <v>91</v>
+      </c>
+      <c r="E92" t="s">
+        <v>2</v>
+      </c>
+      <c r="F92" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A93">
+        <v>92</v>
+      </c>
+      <c r="B93" t="s">
+        <v>2</v>
+      </c>
+      <c r="C93" s="1">
+        <v>2</v>
+      </c>
+      <c r="D93">
+        <v>92</v>
+      </c>
+      <c r="E93" t="s">
+        <v>2</v>
+      </c>
+      <c r="F93" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A94">
+        <v>93</v>
+      </c>
+      <c r="B94" t="s">
+        <v>2</v>
+      </c>
+      <c r="C94" s="1">
+        <v>2</v>
+      </c>
+      <c r="D94">
+        <v>93</v>
+      </c>
+      <c r="E94" t="s">
+        <v>2</v>
+      </c>
+      <c r="F94" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A95">
+        <v>94</v>
+      </c>
+      <c r="B95" t="s">
+        <v>2</v>
+      </c>
+      <c r="C95" s="1">
+        <v>2</v>
+      </c>
+      <c r="D95">
+        <v>94</v>
+      </c>
+      <c r="E95" t="s">
+        <v>2</v>
+      </c>
+      <c r="F95" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A96">
+        <v>95</v>
+      </c>
+      <c r="B96" t="s">
+        <v>2</v>
+      </c>
+      <c r="C96" s="1">
+        <v>2</v>
+      </c>
+      <c r="D96">
+        <v>95</v>
+      </c>
+      <c r="E96" t="s">
+        <v>2</v>
+      </c>
+      <c r="F96" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A97">
+        <v>96</v>
+      </c>
+      <c r="B97" t="s">
+        <v>2</v>
+      </c>
+      <c r="C97" s="1">
+        <v>2</v>
+      </c>
+      <c r="D97">
+        <v>96</v>
+      </c>
+      <c r="E97" t="s">
+        <v>2</v>
+      </c>
+      <c r="F97" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A98">
+        <v>97</v>
+      </c>
+      <c r="B98" t="s">
+        <v>2</v>
+      </c>
+      <c r="C98" s="1">
+        <v>2</v>
+      </c>
+      <c r="D98">
+        <v>97</v>
+      </c>
+      <c r="E98" t="s">
+        <v>2</v>
+      </c>
+      <c r="F98" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A99">
+        <v>98</v>
+      </c>
+      <c r="B99" t="s">
+        <v>2</v>
+      </c>
+      <c r="C99" s="1">
+        <v>2</v>
+      </c>
+      <c r="D99">
+        <v>98</v>
+      </c>
+      <c r="E99" t="s">
+        <v>2</v>
+      </c>
+      <c r="F99" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A100">
+        <v>99</v>
+      </c>
+      <c r="B100" t="s">
+        <v>2</v>
+      </c>
+      <c r="C100" s="1">
+        <v>2</v>
+      </c>
+      <c r="D100">
+        <v>99</v>
+      </c>
+      <c r="E100" t="s">
+        <v>2</v>
+      </c>
+      <c r="F100" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A101">
+        <v>100</v>
+      </c>
+      <c r="B101" t="s">
+        <v>2</v>
+      </c>
+      <c r="C101" s="1">
+        <v>2</v>
+      </c>
+      <c r="D101">
+        <v>100</v>
+      </c>
+      <c r="E101" t="s">
+        <v>2</v>
+      </c>
+      <c r="F101" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A102">
+        <v>101</v>
+      </c>
+      <c r="B102" t="s">
+        <v>2</v>
+      </c>
+      <c r="C102" s="1">
+        <v>2</v>
+      </c>
+      <c r="D102">
+        <v>101</v>
+      </c>
+      <c r="E102" t="s">
+        <v>2</v>
+      </c>
+      <c r="F102" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A103">
+        <v>102</v>
+      </c>
+      <c r="B103" t="s">
+        <v>2</v>
+      </c>
+      <c r="C103" s="1">
+        <v>2</v>
+      </c>
+      <c r="D103">
+        <v>102</v>
+      </c>
+      <c r="E103" t="s">
+        <v>2</v>
+      </c>
+      <c r="F103" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A104">
+        <v>103</v>
+      </c>
+      <c r="B104" t="s">
+        <v>2</v>
+      </c>
+      <c r="C104" s="1">
+        <v>2</v>
+      </c>
+      <c r="D104">
+        <v>103</v>
+      </c>
+      <c r="E104" t="s">
+        <v>2</v>
+      </c>
+      <c r="F104" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A105">
+        <v>104</v>
+      </c>
+      <c r="B105" t="s">
+        <v>2</v>
+      </c>
+      <c r="C105" s="1">
+        <v>2</v>
+      </c>
+      <c r="D105">
+        <v>104</v>
+      </c>
+      <c r="E105" t="s">
+        <v>2</v>
+      </c>
+      <c r="F105" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A106">
+        <v>105</v>
+      </c>
+      <c r="B106" t="s">
+        <v>2</v>
+      </c>
+      <c r="C106" s="1">
+        <v>2</v>
+      </c>
+      <c r="D106">
+        <v>105</v>
+      </c>
+      <c r="E106" t="s">
+        <v>2</v>
+      </c>
+      <c r="F106" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A107">
+        <v>106</v>
+      </c>
+      <c r="B107" t="s">
+        <v>2</v>
+      </c>
+      <c r="C107" s="1">
+        <v>2</v>
+      </c>
+      <c r="D107">
+        <v>106</v>
+      </c>
+      <c r="E107" t="s">
+        <v>2</v>
+      </c>
+      <c r="F107" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A108">
+        <v>107</v>
+      </c>
+      <c r="B108" t="s">
+        <v>2</v>
+      </c>
+      <c r="C108" s="1">
+        <v>2</v>
+      </c>
+      <c r="D108">
+        <v>107</v>
+      </c>
+      <c r="E108" t="s">
+        <v>2</v>
+      </c>
+      <c r="F108" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A109">
+        <v>108</v>
+      </c>
+      <c r="B109" t="s">
+        <v>2</v>
+      </c>
+      <c r="C109" s="1">
+        <v>2</v>
+      </c>
+      <c r="D109">
+        <v>108</v>
+      </c>
+      <c r="E109" t="s">
+        <v>2</v>
+      </c>
+      <c r="F109" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A110">
+        <v>109</v>
+      </c>
+      <c r="B110" t="s">
+        <v>2</v>
+      </c>
+      <c r="C110" s="1">
+        <v>2</v>
+      </c>
+      <c r="D110">
+        <v>109</v>
+      </c>
+      <c r="E110" t="s">
+        <v>2</v>
+      </c>
+      <c r="F110" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A111">
+        <v>110</v>
+      </c>
+      <c r="B111" t="s">
+        <v>2</v>
+      </c>
+      <c r="C111" s="1">
+        <v>2</v>
+      </c>
+      <c r="D111">
+        <v>110</v>
+      </c>
+      <c r="E111" t="s">
+        <v>2</v>
+      </c>
+      <c r="F111" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A112">
+        <v>111</v>
+      </c>
+      <c r="B112" t="s">
+        <v>2</v>
+      </c>
+      <c r="C112" s="1">
+        <v>2</v>
+      </c>
+      <c r="D112">
+        <v>111</v>
+      </c>
+      <c r="E112" t="s">
+        <v>2</v>
+      </c>
+      <c r="F112" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A113">
+        <v>112</v>
+      </c>
+      <c r="B113" t="s">
+        <v>2</v>
+      </c>
+      <c r="C113" s="1">
+        <v>2</v>
+      </c>
+      <c r="D113">
+        <v>112</v>
+      </c>
+      <c r="E113" t="s">
+        <v>2</v>
+      </c>
+      <c r="F113" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A114">
+        <v>113</v>
+      </c>
+      <c r="B114" t="s">
+        <v>4</v>
+      </c>
+      <c r="C114" s="1">
+        <v>1</v>
+      </c>
+      <c r="D114">
+        <v>113</v>
+      </c>
+      <c r="E114" t="s">
+        <v>6</v>
+      </c>
+      <c r="F114" s="1">
+        <v>3</v>
+      </c>
+      <c r="G114" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A115">
+        <v>114</v>
+      </c>
+      <c r="B115" t="s">
+        <v>4</v>
+      </c>
+      <c r="C115" s="1">
+        <v>1</v>
+      </c>
+      <c r="D115">
+        <v>114</v>
+      </c>
+      <c r="E115" t="s">
+        <v>4</v>
+      </c>
+      <c r="F115" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A116">
+        <v>115</v>
+      </c>
+      <c r="B116" t="s">
+        <v>4</v>
+      </c>
+      <c r="C116" s="1">
+        <v>1</v>
+      </c>
+      <c r="D116">
+        <v>115</v>
+      </c>
+      <c r="E116" t="s">
+        <v>4</v>
+      </c>
+      <c r="F116" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A117">
+        <v>116</v>
+      </c>
+      <c r="B117" t="s">
+        <v>2</v>
+      </c>
+      <c r="C117" s="1">
+        <v>2</v>
+      </c>
+      <c r="D117">
+        <v>116</v>
+      </c>
+      <c r="E117" t="s">
+        <v>2</v>
+      </c>
+      <c r="F117" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A118">
+        <v>117</v>
+      </c>
+      <c r="B118" t="s">
+        <v>2</v>
+      </c>
+      <c r="C118" s="1">
+        <v>2</v>
+      </c>
+      <c r="D118">
+        <v>117</v>
+      </c>
+      <c r="E118" t="s">
+        <v>2</v>
+      </c>
+      <c r="F118" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A119">
+        <v>118</v>
+      </c>
+      <c r="B119" t="s">
+        <v>2</v>
+      </c>
+      <c r="C119" s="1">
+        <v>2</v>
+      </c>
+      <c r="D119">
+        <v>118</v>
+      </c>
+      <c r="E119" t="s">
+        <v>2</v>
+      </c>
+      <c r="F119" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A120">
+        <v>119</v>
+      </c>
+      <c r="B120" t="s">
+        <v>2</v>
+      </c>
+      <c r="C120" s="1">
+        <v>2</v>
+      </c>
+      <c r="D120">
+        <v>119</v>
+      </c>
+      <c r="E120" t="s">
+        <v>2</v>
+      </c>
+      <c r="F120" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A121">
+        <v>120</v>
+      </c>
+      <c r="B121" t="s">
+        <v>2</v>
+      </c>
+      <c r="C121" s="1">
+        <v>2</v>
+      </c>
+      <c r="D121">
+        <v>120</v>
+      </c>
+      <c r="E121" t="s">
+        <v>2</v>
+      </c>
+      <c r="F121" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A122">
+        <v>121</v>
+      </c>
+      <c r="B122" t="s">
+        <v>2</v>
+      </c>
+      <c r="C122" s="1">
+        <v>2</v>
+      </c>
+      <c r="D122">
+        <v>121</v>
+      </c>
+      <c r="E122" t="s">
+        <v>2</v>
+      </c>
+      <c r="F122" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A123">
+        <v>122</v>
+      </c>
+      <c r="B123" t="s">
+        <v>2</v>
+      </c>
+      <c r="C123" s="1">
+        <v>2</v>
+      </c>
+      <c r="D123">
+        <v>122</v>
+      </c>
+      <c r="E123" t="s">
+        <v>2</v>
+      </c>
+      <c r="F123" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A124">
+        <v>123</v>
+      </c>
+      <c r="B124" t="s">
+        <v>2</v>
+      </c>
+      <c r="C124" s="1">
+        <v>2</v>
+      </c>
+      <c r="D124">
+        <v>123</v>
+      </c>
+      <c r="E124" t="s">
+        <v>2</v>
+      </c>
+      <c r="F124" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A125">
+        <v>124</v>
+      </c>
+      <c r="B125" t="s">
+        <v>2</v>
+      </c>
+      <c r="C125" s="1">
+        <v>2</v>
+      </c>
+      <c r="D125">
+        <v>124</v>
+      </c>
+      <c r="E125" t="s">
+        <v>2</v>
+      </c>
+      <c r="F125" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A126">
+        <v>125</v>
+      </c>
+      <c r="B126" t="s">
+        <v>2</v>
+      </c>
+      <c r="C126" s="1">
+        <v>2</v>
+      </c>
+      <c r="D126">
+        <v>125</v>
+      </c>
+      <c r="E126" t="s">
+        <v>2</v>
+      </c>
+      <c r="F126" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A127">
+        <v>126</v>
+      </c>
+      <c r="B127" t="s">
+        <v>2</v>
+      </c>
+      <c r="C127" s="1">
+        <v>2</v>
+      </c>
+      <c r="D127">
+        <v>126</v>
+      </c>
+      <c r="E127" t="s">
+        <v>2</v>
+      </c>
+      <c r="F127" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A128">
+        <v>127</v>
+      </c>
+      <c r="B128" t="s">
+        <v>2</v>
+      </c>
+      <c r="C128" s="1">
+        <v>2</v>
+      </c>
+      <c r="D128">
+        <v>127</v>
+      </c>
+      <c r="E128" t="s">
+        <v>2</v>
+      </c>
+      <c r="F128" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A129">
+        <v>128</v>
+      </c>
+      <c r="B129" t="s">
+        <v>2</v>
+      </c>
+      <c r="C129" s="1">
+        <v>2</v>
+      </c>
+      <c r="D129">
+        <v>128</v>
+      </c>
+      <c r="E129" t="s">
+        <v>2</v>
+      </c>
+      <c r="F129" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A130">
+        <v>129</v>
+      </c>
+      <c r="B130" t="s">
+        <v>2</v>
+      </c>
+      <c r="C130" s="1">
+        <v>2</v>
+      </c>
+      <c r="D130">
+        <v>129</v>
+      </c>
+      <c r="E130" t="s">
+        <v>4</v>
+      </c>
+      <c r="F130" s="1">
+        <v>1</v>
+      </c>
+      <c r="G130" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A131">
+        <v>130</v>
+      </c>
+      <c r="B131" t="s">
+        <v>4</v>
+      </c>
+      <c r="C131" s="1">
+        <v>1</v>
+      </c>
+      <c r="D131">
+        <v>130</v>
+      </c>
+      <c r="E131" t="s">
+        <v>4</v>
+      </c>
+      <c r="F131" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A132">
+        <v>131</v>
+      </c>
+      <c r="B132" t="s">
+        <v>4</v>
+      </c>
+      <c r="C132" s="1">
+        <v>1</v>
+      </c>
+      <c r="D132">
+        <v>131</v>
+      </c>
+      <c r="E132" t="s">
+        <v>6</v>
+      </c>
+      <c r="F132" s="1">
+        <v>3</v>
+      </c>
+      <c r="G132" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A133">
+        <v>132</v>
+      </c>
+      <c r="B133" t="s">
+        <v>6</v>
+      </c>
+      <c r="C133" s="1">
+        <v>3</v>
+      </c>
+      <c r="D133">
+        <v>132</v>
+      </c>
+      <c r="E133" t="s">
+        <v>6</v>
+      </c>
+      <c r="F133" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A134">
+        <v>133</v>
+      </c>
+      <c r="B134" t="s">
+        <v>4</v>
+      </c>
+      <c r="C134" s="1">
+        <v>1</v>
+      </c>
+      <c r="D134">
+        <v>133</v>
+      </c>
+      <c r="E134" t="s">
+        <v>4</v>
+      </c>
+      <c r="F134" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A135">
+        <v>134</v>
+      </c>
+      <c r="B135" t="s">
+        <v>4</v>
+      </c>
+      <c r="C135" s="1">
+        <v>1</v>
+      </c>
+      <c r="D135">
+        <v>134</v>
+      </c>
+      <c r="E135" t="s">
+        <v>6</v>
+      </c>
+      <c r="F135" s="1">
+        <v>3</v>
+      </c>
+      <c r="G135" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A136">
+        <v>135</v>
+      </c>
+      <c r="B136" t="s">
+        <v>2</v>
+      </c>
+      <c r="C136" s="1">
+        <v>2</v>
+      </c>
+      <c r="D136">
+        <v>135</v>
+      </c>
+      <c r="E136" t="s">
+        <v>2</v>
+      </c>
+      <c r="F136" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="137" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A137">
+        <v>136</v>
+      </c>
+      <c r="B137" t="s">
+        <v>4</v>
+      </c>
+      <c r="C137" s="1">
+        <v>1</v>
+      </c>
+      <c r="D137">
+        <v>136</v>
+      </c>
+      <c r="E137" t="s">
+        <v>4</v>
+      </c>
+      <c r="F137" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A138">
+        <v>137</v>
+      </c>
+      <c r="B138" t="s">
+        <v>4</v>
+      </c>
+      <c r="C138" s="1">
+        <v>1</v>
+      </c>
+      <c r="D138">
+        <v>137</v>
+      </c>
+      <c r="E138" t="s">
+        <v>4</v>
+      </c>
+      <c r="F138" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A139">
+        <v>138</v>
+      </c>
+      <c r="B139" t="s">
+        <v>4</v>
+      </c>
+      <c r="C139" s="1">
+        <v>1</v>
+      </c>
+      <c r="D139">
+        <v>138</v>
+      </c>
+      <c r="E139" t="s">
+        <v>2</v>
+      </c>
+      <c r="F139" s="1">
+        <v>2</v>
+      </c>
+      <c r="G139" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A140">
+        <v>139</v>
+      </c>
+      <c r="B140" t="s">
+        <v>4</v>
+      </c>
+      <c r="C140" s="1">
+        <v>1</v>
+      </c>
+      <c r="D140">
+        <v>139</v>
+      </c>
+      <c r="E140" t="s">
+        <v>2</v>
+      </c>
+      <c r="F140" s="1">
+        <v>2</v>
+      </c>
+      <c r="G140" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A141">
+        <v>140</v>
+      </c>
+      <c r="B141" t="s">
+        <v>2</v>
+      </c>
+      <c r="C141" s="1">
+        <v>2</v>
+      </c>
+      <c r="D141">
+        <v>140</v>
+      </c>
+      <c r="E141" t="s">
+        <v>2</v>
+      </c>
+      <c r="F141" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="142" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A142">
+        <v>141</v>
+      </c>
+      <c r="B142" t="s">
+        <v>2</v>
+      </c>
+      <c r="C142" s="1">
+        <v>2</v>
+      </c>
+      <c r="D142">
+        <v>141</v>
+      </c>
+      <c r="E142" t="s">
+        <v>2</v>
+      </c>
+      <c r="F142" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A143">
+        <v>142</v>
+      </c>
+      <c r="B143" t="s">
+        <v>2</v>
+      </c>
+      <c r="C143" s="1">
+        <v>2</v>
+      </c>
+      <c r="D143">
+        <v>142</v>
+      </c>
+      <c r="E143" t="s">
+        <v>2</v>
+      </c>
+      <c r="F143" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A144">
+        <v>143</v>
+      </c>
+      <c r="B144" t="s">
+        <v>4</v>
+      </c>
+      <c r="C144" s="1">
+        <v>1</v>
+      </c>
+      <c r="D144">
+        <v>143</v>
+      </c>
+      <c r="E144" t="s">
+        <v>2</v>
+      </c>
+      <c r="F144" s="1">
+        <v>2</v>
+      </c>
+      <c r="G144" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="145" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A145">
+        <v>144</v>
+      </c>
+      <c r="B145" t="s">
+        <v>4</v>
+      </c>
+      <c r="C145" s="1">
+        <v>1</v>
+      </c>
+      <c r="D145">
+        <v>144</v>
+      </c>
+      <c r="E145" t="s">
+        <v>6</v>
+      </c>
+      <c r="F145" s="1">
+        <v>3</v>
+      </c>
+      <c r="G145" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="146" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A146">
+        <v>145</v>
+      </c>
+      <c r="B146" t="s">
+        <v>4</v>
+      </c>
+      <c r="C146" s="1">
+        <v>1</v>
+      </c>
+      <c r="D146">
+        <v>145</v>
+      </c>
+      <c r="E146" t="s">
+        <v>4</v>
+      </c>
+      <c r="F146" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="147" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A147">
+        <v>146</v>
+      </c>
+      <c r="B147" t="s">
+        <v>4</v>
+      </c>
+      <c r="C147" s="1">
+        <v>1</v>
+      </c>
+      <c r="D147">
+        <v>146</v>
+      </c>
+      <c r="E147" t="s">
+        <v>4</v>
+      </c>
+      <c r="F147" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="148" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A148">
+        <v>147</v>
+      </c>
+      <c r="B148" t="s">
+        <v>6</v>
+      </c>
+      <c r="C148" s="1">
+        <v>3</v>
+      </c>
+      <c r="D148">
+        <v>147</v>
+      </c>
+      <c r="E148" t="s">
+        <v>6</v>
+      </c>
+      <c r="F148" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="149" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A149">
+        <v>148</v>
+      </c>
+      <c r="B149" t="s">
+        <v>3</v>
+      </c>
+      <c r="C149" s="1">
+        <v>4</v>
+      </c>
+      <c r="D149">
+        <v>148</v>
+      </c>
+      <c r="E149" t="s">
+        <v>3</v>
+      </c>
+      <c r="F149" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="150" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A150">
+        <v>149</v>
+      </c>
+      <c r="B150" t="s">
+        <v>4</v>
+      </c>
+      <c r="C150" s="1">
+        <v>1</v>
+      </c>
+      <c r="D150">
+        <v>149</v>
+      </c>
+      <c r="E150" t="s">
+        <v>4</v>
+      </c>
+      <c r="F150" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="151" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A151">
+        <v>150</v>
+      </c>
+      <c r="B151" t="s">
+        <v>5</v>
+      </c>
+      <c r="C151" s="1">
+        <v>7</v>
+      </c>
+      <c r="D151">
+        <v>150</v>
+      </c>
+      <c r="E151" t="s">
+        <v>6</v>
+      </c>
+      <c r="F151" s="1">
+        <v>3</v>
+      </c>
+      <c r="G151" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="152" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A152">
+        <v>151</v>
+      </c>
+      <c r="B152" t="s">
+        <v>4</v>
+      </c>
+      <c r="C152" s="1">
+        <v>1</v>
+      </c>
+      <c r="D152">
+        <v>151</v>
+      </c>
+      <c r="E152" t="s">
+        <v>4</v>
+      </c>
+      <c r="F152" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="153" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A153">
+        <v>152</v>
+      </c>
+      <c r="B153" t="s">
+        <v>4</v>
+      </c>
+      <c r="C153" s="1">
+        <v>1</v>
+      </c>
+      <c r="D153">
+        <v>152</v>
+      </c>
+      <c r="E153" t="s">
+        <v>4</v>
+      </c>
+      <c r="F153" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="154" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A154">
+        <v>153</v>
+      </c>
+      <c r="B154" t="s">
+        <v>6</v>
+      </c>
+      <c r="C154" s="1">
+        <v>3</v>
+      </c>
+      <c r="D154">
+        <v>153</v>
+      </c>
+      <c r="E154" t="s">
+        <v>6</v>
+      </c>
+      <c r="F154" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="155" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A155">
+        <v>154</v>
+      </c>
+      <c r="B155" t="s">
+        <v>4</v>
+      </c>
+      <c r="C155" s="1">
+        <v>1</v>
+      </c>
+      <c r="D155">
+        <v>154</v>
+      </c>
+      <c r="E155" t="s">
+        <v>4</v>
+      </c>
+      <c r="F155" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="156" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A156">
+        <v>155</v>
+      </c>
+      <c r="B156" t="s">
+        <v>2</v>
+      </c>
+      <c r="C156" s="1">
+        <v>2</v>
+      </c>
+      <c r="D156">
+        <v>155</v>
+      </c>
+      <c r="E156" t="s">
+        <v>4</v>
+      </c>
+      <c r="F156" s="1">
+        <v>1</v>
+      </c>
+      <c r="G156" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="157" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A157">
+        <v>156</v>
+      </c>
+      <c r="B157" t="s">
+        <v>0</v>
+      </c>
+      <c r="C157" s="1">
+        <v>6</v>
+      </c>
+      <c r="D157">
+        <v>156</v>
+      </c>
+      <c r="E157" t="s">
+        <v>0</v>
+      </c>
+      <c r="F157" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="158" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A158">
+        <v>157</v>
+      </c>
+      <c r="B158" t="s">
+        <v>3</v>
+      </c>
+      <c r="C158" s="1">
+        <v>4</v>
+      </c>
+      <c r="D158">
+        <v>157</v>
+      </c>
+      <c r="E158" t="s">
+        <v>3</v>
+      </c>
+      <c r="F158" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="159" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A159">
+        <v>158</v>
+      </c>
+      <c r="B159" t="s">
+        <v>4</v>
+      </c>
+      <c r="C159" s="1">
+        <v>1</v>
+      </c>
+      <c r="D159">
+        <v>158</v>
+      </c>
+      <c r="E159" t="s">
+        <v>6</v>
+      </c>
+      <c r="F159" s="1">
+        <v>3</v>
+      </c>
+      <c r="G159" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="160" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A160">
+        <v>159</v>
+      </c>
+      <c r="B160" t="s">
+        <v>4</v>
+      </c>
+      <c r="C160" s="1">
+        <v>1</v>
+      </c>
+      <c r="D160">
+        <v>159</v>
+      </c>
+      <c r="E160" t="s">
+        <v>4</v>
+      </c>
+      <c r="F160" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="161" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A161">
+        <v>160</v>
+      </c>
+      <c r="B161" t="s">
+        <v>4</v>
+      </c>
+      <c r="C161" s="1">
+        <v>1</v>
+      </c>
+      <c r="D161">
+        <v>160</v>
+      </c>
+      <c r="E161" t="s">
+        <v>4</v>
+      </c>
+      <c r="F161" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="162" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A162">
+        <v>161</v>
+      </c>
+      <c r="B162" t="s">
+        <v>4</v>
+      </c>
+      <c r="C162" s="1">
+        <v>1</v>
+      </c>
+      <c r="D162">
+        <v>161</v>
+      </c>
+      <c r="E162" t="s">
+        <v>4</v>
+      </c>
+      <c r="F162" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="163" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A163">
+        <v>162</v>
+      </c>
+      <c r="B163" t="s">
+        <v>4</v>
+      </c>
+      <c r="C163" s="1">
+        <v>1</v>
+      </c>
+      <c r="D163">
+        <v>162</v>
+      </c>
+      <c r="E163" t="s">
+        <v>4</v>
+      </c>
+      <c r="F163" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="164" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A164">
+        <v>163</v>
+      </c>
+      <c r="B164" t="s">
+        <v>4</v>
+      </c>
+      <c r="C164" s="1">
+        <v>1</v>
+      </c>
+      <c r="D164">
+        <v>163</v>
+      </c>
+      <c r="E164" t="s">
+        <v>6</v>
+      </c>
+      <c r="F164" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="165" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A165">
+        <v>164</v>
+      </c>
+      <c r="B165" t="s">
+        <v>1</v>
+      </c>
+      <c r="C165" s="1">
+        <v>5</v>
+      </c>
+      <c r="D165">
+        <v>164</v>
+      </c>
+      <c r="E165" t="s">
+        <v>1</v>
+      </c>
+      <c r="F165" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="166" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A166">
+        <v>165</v>
+      </c>
+      <c r="B166" t="s">
+        <v>4</v>
+      </c>
+      <c r="C166" s="1">
+        <v>1</v>
+      </c>
+      <c r="D166">
+        <v>165</v>
+      </c>
+      <c r="E166" t="s">
+        <v>4</v>
+      </c>
+      <c r="F166" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="167" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A167">
+        <v>166</v>
+      </c>
+      <c r="B167" t="s">
+        <v>4</v>
+      </c>
+      <c r="C167" s="1">
+        <v>1</v>
+      </c>
+      <c r="D167">
+        <v>166</v>
+      </c>
+      <c r="E167" t="s">
+        <v>4</v>
+      </c>
+      <c r="F167" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="168" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A168">
+        <v>167</v>
+      </c>
+      <c r="B168" t="s">
+        <v>6</v>
+      </c>
+      <c r="C168" s="1">
+        <v>3</v>
+      </c>
+      <c r="D168">
+        <v>167</v>
+      </c>
+      <c r="E168" t="s">
+        <v>6</v>
+      </c>
+      <c r="F168" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="169" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A169">
+        <v>168</v>
+      </c>
+      <c r="B169" t="s">
+        <v>33</v>
+      </c>
+      <c r="C169" s="1">
+        <v>4</v>
+      </c>
+      <c r="D169">
+        <v>168</v>
+      </c>
+      <c r="E169" t="s">
+        <v>3</v>
+      </c>
+      <c r="F169" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="170" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A170">
+        <v>169</v>
+      </c>
+      <c r="B170" t="s">
+        <v>4</v>
+      </c>
+      <c r="C170" s="1">
+        <v>1</v>
+      </c>
+      <c r="D170">
+        <v>169</v>
+      </c>
+      <c r="E170" t="s">
+        <v>3</v>
+      </c>
+      <c r="F170" s="1">
+        <v>4</v>
+      </c>
+      <c r="G170" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="171" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A171">
+        <v>170</v>
+      </c>
+      <c r="B171" t="s">
+        <v>4</v>
+      </c>
+      <c r="C171" s="1">
+        <v>1</v>
+      </c>
+      <c r="D171">
+        <v>170</v>
+      </c>
+      <c r="E171" t="s">
+        <v>4</v>
+      </c>
+      <c r="F171" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="172" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A172">
+        <v>171</v>
+      </c>
+      <c r="B172" t="s">
+        <v>4</v>
+      </c>
+      <c r="C172" s="1">
+        <v>1</v>
+      </c>
+      <c r="D172">
+        <v>171</v>
+      </c>
+      <c r="E172" t="s">
+        <v>4</v>
+      </c>
+      <c r="F172" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="173" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A173">
+        <v>172</v>
+      </c>
+      <c r="B173" t="s">
+        <v>4</v>
+      </c>
+      <c r="C173" s="1">
+        <v>1</v>
+      </c>
+      <c r="D173">
+        <v>172</v>
+      </c>
+      <c r="E173" t="s">
+        <v>4</v>
+      </c>
+      <c r="F173" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="174" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A174">
+        <v>173</v>
+      </c>
+      <c r="B174" t="s">
+        <v>4</v>
+      </c>
+      <c r="C174" s="1">
+        <v>1</v>
+      </c>
+      <c r="D174">
+        <v>173</v>
+      </c>
+      <c r="E174" t="s">
+        <v>4</v>
+      </c>
+      <c r="F174" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="175" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A175">
+        <v>174</v>
+      </c>
+      <c r="B175" t="s">
+        <v>4</v>
+      </c>
+      <c r="C175" s="1">
+        <v>1</v>
+      </c>
+      <c r="D175">
+        <v>174</v>
+      </c>
+      <c r="E175" t="s">
+        <v>4</v>
+      </c>
+      <c r="F175" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="176" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A176">
+        <v>175</v>
+      </c>
+      <c r="B176" t="s">
+        <v>4</v>
+      </c>
+      <c r="C176" s="1">
+        <v>1</v>
+      </c>
+      <c r="D176">
+        <v>175</v>
+      </c>
+      <c r="E176" t="s">
+        <v>4</v>
+      </c>
+      <c r="F176" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="177" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A177">
+        <v>176</v>
+      </c>
+      <c r="B177" t="s">
+        <v>6</v>
+      </c>
+      <c r="C177" s="1">
+        <v>3</v>
+      </c>
+      <c r="D177">
+        <v>176</v>
+      </c>
+      <c r="E177" t="s">
+        <v>6</v>
+      </c>
+      <c r="F177" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="178" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A178">
+        <v>177</v>
+      </c>
+      <c r="B178" t="s">
+        <v>4</v>
+      </c>
+      <c r="C178" s="1">
+        <v>1</v>
+      </c>
+      <c r="D178">
+        <v>177</v>
+      </c>
+      <c r="E178" t="s">
+        <v>4</v>
+      </c>
+      <c r="F178" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="179" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A179">
+        <v>178</v>
+      </c>
+      <c r="B179" t="s">
+        <v>4</v>
+      </c>
+      <c r="C179" s="1">
+        <v>1</v>
+      </c>
+      <c r="D179">
+        <v>178</v>
+      </c>
+      <c r="E179" t="s">
+        <v>4</v>
+      </c>
+      <c r="F179" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="180" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A180">
+        <v>179</v>
+      </c>
+      <c r="B180" t="s">
+        <v>4</v>
+      </c>
+      <c r="C180" s="1">
+        <v>1</v>
+      </c>
+      <c r="D180">
+        <v>179</v>
+      </c>
+      <c r="E180" t="s">
+        <v>4</v>
+      </c>
+      <c r="F180" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="181" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A181">
+        <v>180</v>
+      </c>
+      <c r="B181" t="s">
+        <v>4</v>
+      </c>
+      <c r="C181" s="1">
+        <v>1</v>
+      </c>
+      <c r="D181">
+        <v>180</v>
+      </c>
+      <c r="E181" t="s">
+        <v>4</v>
+      </c>
+      <c r="F181" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="182" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A182">
+        <v>181</v>
+      </c>
+      <c r="B182" t="s">
+        <v>3</v>
+      </c>
+      <c r="C182" s="1">
+        <v>4</v>
+      </c>
+      <c r="D182">
+        <v>181</v>
+      </c>
+      <c r="E182" t="s">
+        <v>3</v>
+      </c>
+      <c r="F182" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="183" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A183">
+        <v>182</v>
+      </c>
+      <c r="B183" t="s">
+        <v>4</v>
+      </c>
+      <c r="C183" s="1">
+        <v>1</v>
+      </c>
+      <c r="D183">
+        <v>182</v>
+      </c>
+      <c r="E183" t="s">
+        <v>4</v>
+      </c>
+      <c r="F183" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="184" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A184">
+        <v>183</v>
+      </c>
+      <c r="B184" t="s">
+        <v>4</v>
+      </c>
+      <c r="C184" s="1">
+        <v>1</v>
+      </c>
+      <c r="D184">
+        <v>183</v>
+      </c>
+      <c r="E184" t="s">
+        <v>4</v>
+      </c>
+      <c r="F184" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="185" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A185">
+        <v>184</v>
+      </c>
+      <c r="B185" t="s">
+        <v>3</v>
+      </c>
+      <c r="C185" s="1">
+        <v>4</v>
+      </c>
+      <c r="D185">
+        <v>184</v>
+      </c>
+      <c r="E185" t="s">
+        <v>3</v>
+      </c>
+      <c r="F185" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="186" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A186">
+        <v>185</v>
+      </c>
+      <c r="B186" t="s">
+        <v>4</v>
+      </c>
+      <c r="C186" s="1">
+        <v>1</v>
+      </c>
+      <c r="D186">
+        <v>185</v>
+      </c>
+      <c r="E186" t="s">
+        <v>4</v>
+      </c>
+      <c r="F186" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="187" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A187">
+        <v>186</v>
+      </c>
+      <c r="B187" t="s">
+        <v>6</v>
+      </c>
+      <c r="C187" s="1">
+        <v>3</v>
+      </c>
+      <c r="D187">
+        <v>186</v>
+      </c>
+      <c r="E187" t="s">
+        <v>6</v>
+      </c>
+      <c r="F187" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="188" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A188">
+        <v>187</v>
+      </c>
+      <c r="B188" t="s">
+        <v>6</v>
+      </c>
+      <c r="C188" s="1">
+        <v>3</v>
+      </c>
+      <c r="D188">
+        <v>187</v>
+      </c>
+      <c r="E188" t="s">
+        <v>6</v>
+      </c>
+      <c r="F188" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="189" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G189">
+        <f>COUNTA(G2:G188)</f>
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Aug 23 General File Cleanup
Clean out old files.
</commit_message>
<xml_diff>
--- a/Testing/DBvKG Comparison.xlsx
+++ b/Testing/DBvKG Comparison.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19300" tabRatio="500" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19280" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="4" r:id="rId1"/>
@@ -67,7 +67,7 @@
     </textPr>
   </connection>
   <connection id="4" name="DDB5" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" sourceFile="/Users/gradyke/Documents/GitHub/LegalTreebankDev/Testing/DDB5.csv" comma="1">
+    <textPr fileType="mac" sourceFile="/Users/gradyke/Documents/GitHub/LegalTreebankDev/Testing/DDB5.csv" comma="1">
       <textFields count="2">
         <textField/>
         <textField/>
@@ -83,7 +83,7 @@
     </textPr>
   </connection>
   <connection id="6" name="KAG5" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" sourceFile="/Users/gradyke/Documents/GitHub/LegalTreebankDev/Testing/KAG5.csv" comma="1">
+    <textPr fileType="mac" sourceFile="/Users/gradyke/Documents/GitHub/LegalTreebankDev/Testing/KAG5.csv" comma="1">
       <textFields count="2">
         <textField/>
         <textField/>
@@ -94,7 +94,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1483" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1505" uniqueCount="49">
   <si>
     <t xml:space="preserve"> procedure</t>
   </si>
@@ -200,6 +200,48 @@
   <si>
     <t>analysis</t>
   </si>
+  <si>
+    <t>Number of Sentence Tokens</t>
+  </si>
+  <si>
+    <t>Case Number</t>
+  </si>
+  <si>
+    <t>000001</t>
+  </si>
+  <si>
+    <t>000002</t>
+  </si>
+  <si>
+    <t>000003</t>
+  </si>
+  <si>
+    <t>000004</t>
+  </si>
+  <si>
+    <t>000005</t>
+  </si>
+  <si>
+    <t>000006</t>
+  </si>
+  <si>
+    <t>000007</t>
+  </si>
+  <si>
+    <t>000008</t>
+  </si>
+  <si>
+    <t>000009</t>
+  </si>
+  <si>
+    <t>000010</t>
+  </si>
+  <si>
+    <t>Cohen's K</t>
+  </si>
+  <si>
+    <t>Final</t>
+  </si>
 </sst>
 </file>
 
@@ -264,7 +306,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -275,6 +317,9 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -304,11 +349,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="KAG_1" connectionId="5" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DDB_1" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DDB_1" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="KAG_1" connectionId="5" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
@@ -582,22 +627,108 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="168" zoomScaleNormal="168" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="24.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P214"/>
+  <dimension ref="A1:S214"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O7" sqref="O7"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -610,7 +741,7 @@
     <col min="16" max="16" width="23.33203125" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>28</v>
       </c>
@@ -632,8 +763,14 @@
       <c r="K1" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="R1" t="s">
+        <v>11</v>
+      </c>
+      <c r="S1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -668,7 +805,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -704,7 +841,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -740,7 +877,7 @@
         <v>0.77934272300469487</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -769,7 +906,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -807,7 +944,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -847,7 +984,7 @@
         <v>0.40952380952380951</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -887,7 +1024,7 @@
         <v>0.23809523809523808</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -927,7 +1064,7 @@
         <v>8.0952380952380956E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -967,7 +1104,7 @@
         <v>5.2380952380952382E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1007,7 +1144,7 @@
         <v>8.5714285714285715E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1047,7 +1184,7 @@
         <v>5.2380952380952382E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1087,7 +1224,7 @@
         <v>8.0952380952380956E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1124,7 +1261,7 @@
         <v>1.502758214483582E-7</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1153,7 +1290,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -7106,7 +7243,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K153"/>
   <sheetViews>
-    <sheetView topLeftCell="A146" zoomScale="184" zoomScaleNormal="184" workbookViewId="0">
+    <sheetView zoomScale="184" zoomScaleNormal="184" workbookViewId="0">
       <selection activeCell="G153" sqref="G153"/>
     </sheetView>
   </sheetViews>
@@ -14573,7 +14710,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="124" zoomScaleNormal="124" workbookViewId="0">
+    <sheetView topLeftCell="A14" zoomScale="124" zoomScaleNormal="124" workbookViewId="0">
       <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>

</xml_diff>